<commit_message>
Made username and password in commands file generic
</commit_message>
<xml_diff>
--- a/test-excel-file.xlsx
+++ b/test-excel-file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattg\Documents\GitHub\aim-bot-prototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585F8190-4804-4C9F-BB69-FC619E514CDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54511780-4ECF-482F-AAF4-AB9DFEFD730F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="20">
   <si>
     <t>Command</t>
   </si>
@@ -72,9 +72,6 @@
     <t>c</t>
   </si>
   <si>
-    <t>gracz</t>
-  </si>
-  <si>
     <t>mainForm:browse:0:ae_s_sec_c_login</t>
   </si>
   <si>
@@ -82,6 +79,12 @@
   </si>
   <si>
     <t>mattsNewPassword!</t>
+  </si>
+  <si>
+    <t>&lt;username&gt;</t>
+  </si>
+  <si>
+    <t>&lt;password&gt;</t>
   </si>
 </sst>
 </file>
@@ -414,7 +417,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,7 +481,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -494,7 +497,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -507,7 +510,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -521,7 +524,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Major refactor partially done, just stashing code
</commit_message>
<xml_diff>
--- a/test-excel-file.xlsx
+++ b/test-excel-file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattg\Documents\GitHub\aim-bot-prototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54511780-4ECF-482F-AAF4-AB9DFEFD730F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994D303D-FBF9-41F4-9A2A-87F83AFCE178}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Command</t>
   </si>
@@ -78,13 +78,10 @@
     <t>Clear</t>
   </si>
   <si>
-    <t>mattsNewPassword!</t>
-  </si>
-  <si>
-    <t>&lt;username&gt;</t>
-  </si>
-  <si>
-    <t>&lt;password&gt;</t>
+    <t>gracz</t>
+  </si>
+  <si>
+    <t>passwerd</t>
   </si>
 </sst>
 </file>
@@ -417,7 +414,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +478,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -524,7 +521,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>